<commit_message>
compulsory booklet some scenarios added
</commit_message>
<xml_diff>
--- a/Compulsory_booklet_PyQt_NPS.xlsx
+++ b/Compulsory_booklet_PyQt_NPS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\014_migration_NPS_to_PyQt\NPS_PyQt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7E1C8C50-42EA-4446-8C7D-7B37E7AE18C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9362BBEA-4EF0-4BCF-A8CC-8B7CBC2AA8D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7794DAE8-CD6E-4545-94BD-4013928028B0}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>Widget</t>
   </si>
@@ -83,6 +83,18 @@
   </si>
   <si>
     <t>moved</t>
+  </si>
+  <si>
+    <t>scroll</t>
+  </si>
+  <si>
+    <t>radio buttons</t>
+  </si>
+  <si>
+    <t>checked</t>
+  </si>
+  <si>
+    <t>switch between ROI selection modes</t>
   </si>
 </sst>
 </file>
@@ -434,10 +446,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C325169-7AAD-4C53-BAC4-A988129FC781}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -513,6 +525,22 @@
         <v>15</v>
       </c>
     </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
compulsory booklet edited, some auxiliary files to figure out how to use QRubberBand
</commit_message>
<xml_diff>
--- a/Compulsory_booklet_PyQt_NPS.xlsx
+++ b/Compulsory_booklet_PyQt_NPS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\014_migration_NPS_to_PyQt\NPS_PyQt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9362BBEA-4EF0-4BCF-A8CC-8B7CBC2AA8D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62DB1DD3-3895-4264-B15A-058484C1B60D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7794DAE8-CD6E-4545-94BD-4013928028B0}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="35">
   <si>
     <t>Widget</t>
   </si>
@@ -95,6 +95,51 @@
   </si>
   <si>
     <t>switch between ROI selection modes</t>
+  </si>
+  <si>
+    <t>ROI array radio button</t>
+  </si>
+  <si>
+    <t>Open a dialog window</t>
+  </si>
+  <si>
+    <t>erase last ROI</t>
+  </si>
+  <si>
+    <t>create resulting XLSX</t>
+  </si>
+  <si>
+    <t>processLabel</t>
+  </si>
+  <si>
+    <t>show the function/method/process which is being executed</t>
+  </si>
+  <si>
+    <t>class name</t>
+  </si>
+  <si>
+    <t>method name</t>
+  </si>
+  <si>
+    <t>line</t>
+  </si>
+  <si>
+    <t>GUI</t>
+  </si>
+  <si>
+    <t>motion</t>
+  </si>
+  <si>
+    <t>slide_images</t>
+  </si>
+  <si>
+    <t>to be added</t>
+  </si>
+  <si>
+    <t>draw</t>
+  </si>
+  <si>
+    <t>erase_last</t>
   </si>
 </sst>
 </file>
@@ -446,18 +491,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C325169-7AAD-4C53-BAC4-A988129FC781}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="30.28515625" customWidth="1"/>
+    <col min="1" max="3" width="30.28515625" customWidth="1"/>
+    <col min="4" max="4" width="55.5703125" customWidth="1"/>
+    <col min="5" max="5" width="32.85546875" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -470,8 +518,17 @@
       <c r="D1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -481,8 +538,17 @@
       <c r="D2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G2">
+        <v>1824</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>6</v>
       </c>
@@ -492,16 +558,31 @@
       <c r="D3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>8</v>
       </c>
       <c r="D4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G4">
+        <v>2028</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>9</v>
       </c>
@@ -509,7 +590,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>10</v>
       </c>
@@ -517,20 +598,32 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>14</v>
       </c>
       <c r="C7" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G7">
+        <v>1848</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>17</v>
       </c>
@@ -539,6 +632,41 @@
       </c>
       <c r="D9" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11" t="s">
+        <v>34</v>
+      </c>
+      <c r="G11">
+        <v>2175</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>